<commit_message>
[IMP] extras: Improve about page and poetry pdf file.
</commit_message>
<xml_diff>
--- a/app/extras/data_xls/poetry_dig_lib_xlsx.xlsx
+++ b/app/extras/data_xls/poetry_dig_lib_xlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joanp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\repos\poetry-lib-explorer\app\extras\data_xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D930914-055E-420A-AF58-10D1BDD0E345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A185864-8DC3-4FC6-BDCA-DC775346FF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,9 +134,6 @@
 como si estuviera aún
 en vilo. 
 </t>
-  </si>
-  <si>
-    <t>Pequeño y humilde colección de poemas Vol. I (Spanish)</t>
   </si>
   <si>
     <t>El atardecer devolvió a mi corazón la primavera</t>
@@ -1088,9 +1085,6 @@
 </t>
   </si>
   <si>
-    <t>Pequeño y humilde colección de poemas Vol. II (Spanish)</t>
-  </si>
-  <si>
     <t>El eco de tus risas</t>
   </si>
   <si>
@@ -1520,6 +1514,12 @@
 con mi gente y sus costumbres, 
 pero  no es París.
 </t>
+  </si>
+  <si>
+    <t>Pequeña y humilde colección de poemas Vol. I (Spanish)</t>
+  </si>
+  <si>
+    <t>Pequeña y humilde colección de poemas Vol. II (Spanish)</t>
   </si>
 </sst>
 </file>
@@ -2008,7 +2008,7 @@
         <v>28</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>26</v>
@@ -2052,7 +2052,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -2070,10 +2070,10 @@
         <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>26</v>
@@ -2117,7 +2117,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -2135,10 +2135,10 @@
         <v>27</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>26</v>
@@ -2182,7 +2182,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>26</v>
@@ -2200,10 +2200,10 @@
         <v>27</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>26</v>
@@ -2229,7 +2229,7 @@
         <v>45318.045695589317</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -2249,7 +2249,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -2267,10 +2267,10 @@
         <v>27</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>26</v>
@@ -2314,7 +2314,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>26</v>
@@ -2332,10 +2332,10 @@
         <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>26</v>
@@ -2379,7 +2379,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>26</v>
@@ -2397,10 +2397,10 @@
         <v>27</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>26</v>
@@ -2426,7 +2426,7 @@
         <v>45318.045695577763</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -2446,7 +2446,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
@@ -2464,10 +2464,10 @@
         <v>27</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>26</v>
@@ -2511,7 +2511,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
@@ -2529,10 +2529,10 @@
         <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>26</v>
@@ -2576,7 +2576,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>26</v>
@@ -2594,10 +2594,10 @@
         <v>27</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>26</v>
@@ -2641,7 +2641,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>
@@ -2659,10 +2659,10 @@
         <v>27</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>26</v>
@@ -2706,7 +2706,7 @@
         <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>26</v>
@@ -2721,13 +2721,13 @@
         <v>225</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="J13" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>26</v>
@@ -2753,7 +2753,7 @@
         <v>45318.045695589317</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -2773,7 +2773,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>26</v>
@@ -2791,10 +2791,10 @@
         <v>27</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>26</v>
@@ -2838,7 +2838,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>26</v>
@@ -2856,10 +2856,10 @@
         <v>27</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>26</v>
@@ -2903,7 +2903,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
@@ -2918,13 +2918,13 @@
         <v>436</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>26</v>
@@ -2968,7 +2968,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>26</v>
@@ -2983,13 +2983,13 @@
         <v>452</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>26</v>
@@ -3033,7 +3033,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>26</v>
@@ -3051,10 +3051,10 @@
         <v>27</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>26</v>
@@ -3080,7 +3080,7 @@
         <v>45318.045695589317</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -3100,7 +3100,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>26</v>
@@ -3118,10 +3118,10 @@
         <v>27</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>26</v>
@@ -3165,7 +3165,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>26</v>
@@ -3183,10 +3183,10 @@
         <v>27</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>26</v>
@@ -3230,7 +3230,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>26</v>
@@ -3248,10 +3248,10 @@
         <v>27</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>26</v>
@@ -3295,7 +3295,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>26</v>
@@ -3313,10 +3313,10 @@
         <v>27</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>26</v>
@@ -3360,7 +3360,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>26</v>
@@ -3378,10 +3378,10 @@
         <v>27</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>26</v>
@@ -3407,7 +3407,7 @@
         <v>45318.045695577763</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W23">
         <v>0</v>
@@ -3427,7 +3427,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>26</v>
@@ -3445,10 +3445,10 @@
         <v>27</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>26</v>
@@ -3474,7 +3474,7 @@
         <v>45318.045695577763</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W24">
         <v>0</v>
@@ -3494,7 +3494,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>26</v>
@@ -3512,10 +3512,10 @@
         <v>27</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>26</v>
@@ -3541,7 +3541,7 @@
         <v>45318.045695577763</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W25">
         <v>0</v>
@@ -3561,7 +3561,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>26</v>
@@ -3579,10 +3579,10 @@
         <v>27</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>26</v>
@@ -3608,7 +3608,7 @@
         <v>45318.045695577763</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W26">
         <v>0</v>
@@ -3628,7 +3628,7 @@
         <v>31</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>26</v>
@@ -3646,10 +3646,10 @@
         <v>27</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>26</v>
@@ -3693,7 +3693,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>26</v>
@@ -3711,10 +3711,10 @@
         <v>27</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>26</v>
@@ -3758,7 +3758,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>26</v>
@@ -3776,10 +3776,10 @@
         <v>27</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>26</v>
@@ -3823,7 +3823,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>26</v>
@@ -3841,10 +3841,10 @@
         <v>27</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>26</v>
@@ -3870,7 +3870,7 @@
         <v>45318.045695589317</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W30">
         <v>0</v>
@@ -3890,7 +3890,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>26</v>
@@ -3908,10 +3908,10 @@
         <v>27</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>26</v>
@@ -3955,7 +3955,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>26</v>
@@ -3973,10 +3973,10 @@
         <v>27</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>26</v>
@@ -4020,7 +4020,7 @@
         <v>43</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>26</v>
@@ -4038,10 +4038,10 @@
         <v>27</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>26</v>
@@ -4085,7 +4085,7 @@
         <v>44</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>26</v>
@@ -4100,13 +4100,13 @@
         <v>365</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>26</v>
@@ -4150,7 +4150,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>26</v>
@@ -4165,13 +4165,13 @@
         <v>765</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>26</v>
@@ -4215,7 +4215,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>26</v>
@@ -4233,10 +4233,10 @@
         <v>27</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>26</v>
@@ -4280,7 +4280,7 @@
         <v>28</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>26</v>
@@ -4298,10 +4298,10 @@
         <v>27</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>26</v>
@@ -4345,7 +4345,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>26</v>
@@ -4363,10 +4363,10 @@
         <v>27</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>26</v>
@@ -4410,7 +4410,7 @@
         <v>34</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>26</v>
@@ -4428,10 +4428,10 @@
         <v>27</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>26</v>
@@ -4475,7 +4475,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>26</v>
@@ -4493,10 +4493,10 @@
         <v>27</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>26</v>
@@ -4540,7 +4540,7 @@
         <v>37</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>26</v>
@@ -4558,10 +4558,10 @@
         <v>27</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>26</v>
@@ -4605,7 +4605,7 @@
         <v>35</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>26</v>
@@ -4623,10 +4623,10 @@
         <v>27</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>26</v>
@@ -4670,7 +4670,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>26</v>
@@ -4685,13 +4685,13 @@
         <v>562</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>26</v>
@@ -4735,7 +4735,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>26</v>
@@ -4750,13 +4750,13 @@
         <v>779</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>26</v>
@@ -4800,7 +4800,7 @@
         <v>41</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>26</v>
@@ -4818,10 +4818,10 @@
         <v>27</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>26</v>
@@ -4865,7 +4865,7 @@
         <v>42</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>26</v>
@@ -4883,10 +4883,10 @@
         <v>27</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>26</v>
@@ -4930,7 +4930,7 @@
         <v>38</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>26</v>
@@ -4948,10 +4948,10 @@
         <v>27</v>
       </c>
       <c r="I47" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
[IMP] Improve resource data.
</commit_message>
<xml_diff>
--- a/app/extras/data_xls/poetry_dig_lib_xlsx.xlsx
+++ b/app/extras/data_xls/poetry_dig_lib_xlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\repos\poetry-lib-explorer\app\extras\data_xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A185864-8DC3-4FC6-BDCA-DC775346FF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5A0B86-A3DA-4B4F-9FDE-F635EB3620B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,6 +134,9 @@
 como si estuviera aún
 en vilo. 
 </t>
+  </si>
+  <si>
+    <t>Pequeña y humilde colección de poemas Vol. I (Spanish)</t>
   </si>
   <si>
     <t>El atardecer devolvió a mi corazón la primavera</t>
@@ -178,7 +181,7 @@
     <t>Amaneceres</t>
   </si>
   <si>
-    <t xml:space="preserve">Ora Somos amaneceres
+    <t xml:space="preserve">Ora somos amaneceres
 pintados con colores infinitos.
 Todos somos amaneceres,
 que poco a poco se deshojan
@@ -194,15 +197,15 @@
 entre mi mano brilla.
 Veo como abril desaparece
 desde el este hacia el oeste.
-Sé que palidece mi reflejo 
-sin esos felices momentos 
+Sé que palidece mi reflejo
+sin esos felices momentos
 de intimidad.
 Mi cabeza se pierde
 en la abadía;
 por sus coloridos cristales
-el sol radía 
+el sol radía
 lo que me dijiste;
-Qué fácil parece todo
+¡Qué fácil parece todo
 cuando tú estás cerca!
 Somos atardeceres
 pintados con sueños infinitos.
@@ -299,7 +302,7 @@
 Un monte pardo se altea
 en la lejanía, y tú lo miras,
 como quien busca reposo;
-y en la mar, soñolienta,
+y en la mar, somnolienta,
 danza, plateada, la Luna.
 Bulevar de acuarela,
 deja que hilen las divas
@@ -333,7 +336,7 @@
   <si>
     <t xml:space="preserve">¿A qué el rocío helado
 sobre mi piel desnuda?,
-¿a qué la dura sombra
+¿A qué la dura sombra
 que me roba el verano?
 Días claros, huidizos,
 ¿adónde están los arroyos,
@@ -647,7 +650,7 @@
 La brisa del alba perla mi piel,
 mientras se estremece
 mi corazón.
-La noche termina, penosa,
+La noche termina,
 muere el ayer,
 ¿seré, solo, más fuerte, 
 con el amanecer?
@@ -965,7 +968,7 @@
 se dibuja una sonrisa de papel.
 Triste muchachita hecha de miel,
 se sienta en la ventana a ver caer 
-hojas frágiles y rojas por doquier.
+frágiles hojas granas.
 Vulnerable como polilla en la llama
 se dibuja una sonrisa de papel.
 Alma de cristal apoyada en la ventana 
@@ -1083,6 +1086,9 @@
 mas siempre vuelven
 cuando llega la noche.
 </t>
+  </si>
+  <si>
+    <t>Pequeña y humilde colección de poemas Vol. II (Spanish)</t>
   </si>
   <si>
     <t>El eco de tus risas</t>
@@ -1191,16 +1197,6 @@
 ¿Dónde tu profunda sonrisa?
 No llores por lo que has perdido
 no lo encontrarás mirando atrás.
-Me pesa el corazón cuando te veo
-con los ojos humedecidos,
-un velo cubriéndote la cara.
-Como si fuese de otro mundo,
-como si no fuese del todo humana.
-Desearía ver felicidad en esos soles,
-otrora resplandecientes de alegría.
-Hay un nuevo amor en mi vida
-y no voy a hacer que sufra.
-Ahora es demasiado tarde para volver.
 Dulce y triste rosa azul
 Hace tiempo perdiste a tu amado.
 Tu cabecita ahora pasea entre sueños,
@@ -1219,7 +1215,7 @@
 Recuerdos llevados por el viento,
 pequeños sueños desvanecidos en la niebla.
 Aquel camino nevado de enero,
-cuando murieron mis esperanzas.
+cuando murieron tus esperanzas.
 Recuerdo las risas en la playa silenciosa, 
 las estrellas viajando, las luces bajo el mar, 
 el asiento de atrás del viejo Seat Ibiza,
@@ -1422,7 +1418,7 @@
 Sí, lo creí.
 Creí saber lo que era un hombre,
 que era toda una mujer,
-que yo nunca fui idiota.
+que yo nunca fui tonta.
 Sí, lo creí.
 Creí que encontraría alguno mejor,
 siempre a punto el fuego en las venas,
@@ -1449,7 +1445,7 @@
 Una vez
 creí saber lo que era un hombre,
 que era toda una mujer,
-que yo nunca fui idiota.
+que yo nunca fui tonta.
 </t>
   </si>
   <si>
@@ -1514,12 +1510,6 @@
 con mi gente y sus costumbres, 
 pero  no es París.
 </t>
-  </si>
-  <si>
-    <t>Pequeña y humilde colección de poemas Vol. I (Spanish)</t>
-  </si>
-  <si>
-    <t>Pequeña y humilde colección de poemas Vol. II (Spanish)</t>
   </si>
 </sst>
 </file>
@@ -1877,12 +1867,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="12.7265625" customWidth="1"/>
     <col min="3" max="3" width="57.7265625" customWidth="1"/>
@@ -1902,7 +1892,7 @@
     <col min="23" max="25" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +1969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>25</v>
       </c>
@@ -2008,7 +1998,7 @@
         <v>28</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>26</v>
@@ -2018,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="O2">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="3">
@@ -2031,7 +2021,7 @@
         <v>38353</v>
       </c>
       <c r="U2" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V2" s="2"/>
       <c r="W2">
@@ -2044,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>20</v>
       </c>
@@ -2052,7 +2042,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -2070,10 +2060,10 @@
         <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>26</v>
@@ -2083,7 +2073,7 @@
         <v>1</v>
       </c>
       <c r="O3">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="3">
@@ -2096,7 +2086,7 @@
         <v>38353</v>
       </c>
       <c r="U3" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3">
@@ -2109,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>12</v>
       </c>
@@ -2117,7 +2107,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -2129,16 +2119,16 @@
         <v>998245</v>
       </c>
       <c r="G4">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>26</v>
@@ -2148,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="O4">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="3">
@@ -2161,7 +2151,7 @@
         <v>38718</v>
       </c>
       <c r="U4" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V4" s="2"/>
       <c r="W4">
@@ -2174,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>34</v>
       </c>
@@ -2182,7 +2172,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>26</v>
@@ -2200,10 +2190,10 @@
         <v>27</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>26</v>
@@ -2213,7 +2203,7 @@
         <v>1</v>
       </c>
       <c r="O5">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="3">
@@ -2226,10 +2216,10 @@
         <v>38718</v>
       </c>
       <c r="U5" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -2241,7 +2231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>24</v>
       </c>
@@ -2249,7 +2239,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -2267,10 +2257,10 @@
         <v>27</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>26</v>
@@ -2280,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="O6">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="3">
@@ -2293,7 +2283,7 @@
         <v>38353</v>
       </c>
       <c r="U6" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V6" s="2"/>
       <c r="W6">
@@ -2306,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>22</v>
       </c>
@@ -2314,7 +2304,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>26</v>
@@ -2332,10 +2322,10 @@
         <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>26</v>
@@ -2345,7 +2335,7 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="3">
@@ -2358,7 +2348,7 @@
         <v>36526</v>
       </c>
       <c r="U7" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V7" s="2"/>
       <c r="W7">
@@ -2371,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2379,7 +2369,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>26</v>
@@ -2391,16 +2381,16 @@
         <v>902587</v>
       </c>
       <c r="G8">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>26</v>
@@ -2410,7 +2400,7 @@
         <v>1</v>
       </c>
       <c r="O8">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="3">
@@ -2423,10 +2413,10 @@
         <v>38353</v>
       </c>
       <c r="U8" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -2438,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>13</v>
       </c>
@@ -2446,7 +2436,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
@@ -2464,10 +2454,10 @@
         <v>27</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>26</v>
@@ -2477,7 +2467,7 @@
         <v>1</v>
       </c>
       <c r="O9">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="3">
@@ -2490,7 +2480,7 @@
         <v>37987</v>
       </c>
       <c r="U9" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V9" s="2"/>
       <c r="W9">
@@ -2503,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>36</v>
       </c>
@@ -2511,7 +2501,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
@@ -2529,10 +2519,10 @@
         <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>26</v>
@@ -2542,7 +2532,7 @@
         <v>1</v>
       </c>
       <c r="O10">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="3">
@@ -2555,7 +2545,7 @@
         <v>36526</v>
       </c>
       <c r="U10" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V10" s="2"/>
       <c r="W10">
@@ -2568,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>30</v>
       </c>
@@ -2576,7 +2566,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>26</v>
@@ -2594,10 +2584,10 @@
         <v>27</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>26</v>
@@ -2607,7 +2597,7 @@
         <v>1</v>
       </c>
       <c r="O11">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="3">
@@ -2620,7 +2610,7 @@
         <v>38718</v>
       </c>
       <c r="U11" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V11" s="2"/>
       <c r="W11">
@@ -2633,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2641,7 +2631,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>
@@ -2659,10 +2649,10 @@
         <v>27</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>26</v>
@@ -2672,7 +2662,7 @@
         <v>1</v>
       </c>
       <c r="O12">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="3">
@@ -2685,7 +2675,7 @@
         <v>36526</v>
       </c>
       <c r="U12" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V12" s="2"/>
       <c r="W12">
@@ -2698,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>31</v>
       </c>
@@ -2706,7 +2696,7 @@
         <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>26</v>
@@ -2721,13 +2711,13 @@
         <v>225</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>26</v>
@@ -2737,7 +2727,7 @@
         <v>1</v>
       </c>
       <c r="O13">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="3">
@@ -2750,10 +2740,10 @@
         <v>39083</v>
       </c>
       <c r="U13" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -2765,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>26</v>
       </c>
@@ -2773,7 +2763,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>26</v>
@@ -2791,10 +2781,10 @@
         <v>27</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>26</v>
@@ -2804,7 +2794,7 @@
         <v>1</v>
       </c>
       <c r="O14">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="3">
@@ -2817,7 +2807,7 @@
         <v>38718</v>
       </c>
       <c r="U14" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V14" s="2"/>
       <c r="W14">
@@ -2830,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>28</v>
       </c>
@@ -2838,7 +2828,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>26</v>
@@ -2856,10 +2846,10 @@
         <v>27</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>26</v>
@@ -2869,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="O15">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="3">
@@ -2882,7 +2872,7 @@
         <v>36526</v>
       </c>
       <c r="U15" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V15" s="2"/>
       <c r="W15">
@@ -2895,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>6</v>
       </c>
@@ -2903,7 +2893,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
@@ -2918,13 +2908,13 @@
         <v>436</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>26</v>
@@ -2947,7 +2937,7 @@
         <v>38353</v>
       </c>
       <c r="U16" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V16" s="2"/>
       <c r="W16">
@@ -2960,7 +2950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2968,7 +2958,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>26</v>
@@ -2983,13 +2973,13 @@
         <v>452</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>26</v>
@@ -3012,7 +3002,7 @@
         <v>38353</v>
       </c>
       <c r="U17" s="3">
-        <v>45318.045695566172</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V17" s="2"/>
       <c r="W17">
@@ -3025,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>33</v>
       </c>
@@ -3033,7 +3023,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>26</v>
@@ -3051,10 +3041,10 @@
         <v>27</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>26</v>
@@ -3064,7 +3054,7 @@
         <v>1</v>
       </c>
       <c r="O18">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="3">
@@ -3077,10 +3067,10 @@
         <v>38353</v>
       </c>
       <c r="U18" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -3092,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>8</v>
       </c>
@@ -3100,7 +3090,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>26</v>
@@ -3118,10 +3108,10 @@
         <v>27</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>26</v>
@@ -3131,7 +3121,7 @@
         <v>1</v>
       </c>
       <c r="O19">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="3">
@@ -3144,7 +3134,7 @@
         <v>36526</v>
       </c>
       <c r="U19" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V19" s="2"/>
       <c r="W19">
@@ -3157,7 +3147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>14</v>
       </c>
@@ -3165,7 +3155,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>26</v>
@@ -3183,10 +3173,10 @@
         <v>27</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>26</v>
@@ -3196,7 +3186,7 @@
         <v>1</v>
       </c>
       <c r="O20">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="3">
@@ -3209,7 +3199,7 @@
         <v>37987</v>
       </c>
       <c r="U20" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V20" s="2"/>
       <c r="W20">
@@ -3222,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>16</v>
       </c>
@@ -3230,7 +3220,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>26</v>
@@ -3248,10 +3238,10 @@
         <v>27</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>26</v>
@@ -3261,7 +3251,7 @@
         <v>1</v>
       </c>
       <c r="O21">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="3">
@@ -3274,7 +3264,7 @@
         <v>36526</v>
       </c>
       <c r="U21" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V21" s="2"/>
       <c r="W21">
@@ -3287,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>9</v>
       </c>
@@ -3295,7 +3285,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>26</v>
@@ -3307,16 +3297,16 @@
         <v>568440</v>
       </c>
       <c r="G22">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>26</v>
@@ -3326,7 +3316,7 @@
         <v>1</v>
       </c>
       <c r="O22">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="3">
@@ -3339,7 +3329,7 @@
         <v>38353</v>
       </c>
       <c r="U22" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V22" s="2"/>
       <c r="W22">
@@ -3352,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>18</v>
       </c>
@@ -3360,7 +3350,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>26</v>
@@ -3378,10 +3368,10 @@
         <v>27</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>26</v>
@@ -3391,7 +3381,7 @@
         <v>1</v>
       </c>
       <c r="O23">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="3">
@@ -3404,10 +3394,10 @@
         <v>38353</v>
       </c>
       <c r="U23" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="W23">
         <v>0</v>
@@ -3419,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>19</v>
       </c>
@@ -3427,7 +3417,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>26</v>
@@ -3445,10 +3435,10 @@
         <v>27</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>26</v>
@@ -3458,7 +3448,7 @@
         <v>1</v>
       </c>
       <c r="O24">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="3">
@@ -3471,10 +3461,10 @@
         <v>38353</v>
       </c>
       <c r="U24" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="W24">
         <v>0</v>
@@ -3486,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>15</v>
       </c>
@@ -3494,7 +3484,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>26</v>
@@ -3512,10 +3502,10 @@
         <v>27</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>26</v>
@@ -3525,7 +3515,7 @@
         <v>1</v>
       </c>
       <c r="O25">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="3">
@@ -3538,10 +3528,10 @@
         <v>38353</v>
       </c>
       <c r="U25" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="W25">
         <v>0</v>
@@ -3553,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>17</v>
       </c>
@@ -3561,7 +3551,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>26</v>
@@ -3579,10 +3569,10 @@
         <v>27</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>26</v>
@@ -3592,7 +3582,7 @@
         <v>1</v>
       </c>
       <c r="O26">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="3">
@@ -3605,10 +3595,10 @@
         <v>38353</v>
       </c>
       <c r="U26" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="W26">
         <v>0</v>
@@ -3620,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>27</v>
       </c>
@@ -3628,7 +3618,7 @@
         <v>31</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>26</v>
@@ -3646,10 +3636,10 @@
         <v>27</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>26</v>
@@ -3659,7 +3649,7 @@
         <v>1</v>
       </c>
       <c r="O27">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="3">
@@ -3672,7 +3662,7 @@
         <v>38718</v>
       </c>
       <c r="U27" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V27" s="2"/>
       <c r="W27">
@@ -3685,7 +3675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>21</v>
       </c>
@@ -3693,7 +3683,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>26</v>
@@ -3711,10 +3701,10 @@
         <v>27</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>26</v>
@@ -3724,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="O28">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="3">
@@ -3737,7 +3727,7 @@
         <v>38353</v>
       </c>
       <c r="U28" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V28" s="2"/>
       <c r="W28">
@@ -3750,7 +3740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>35</v>
       </c>
@@ -3758,7 +3748,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>26</v>
@@ -3776,10 +3766,10 @@
         <v>27</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>26</v>
@@ -3789,7 +3779,7 @@
         <v>1</v>
       </c>
       <c r="O29">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="3">
@@ -3802,7 +3792,7 @@
         <v>38353</v>
       </c>
       <c r="U29" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V29" s="2"/>
       <c r="W29">
@@ -3815,7 +3805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3823,7 +3813,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>26</v>
@@ -3841,10 +3831,10 @@
         <v>27</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>26</v>
@@ -3854,7 +3844,7 @@
         <v>1</v>
       </c>
       <c r="O30">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="3">
@@ -3867,10 +3857,10 @@
         <v>38718</v>
       </c>
       <c r="U30" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="W30">
         <v>0</v>
@@ -3882,7 +3872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>11</v>
       </c>
@@ -3890,7 +3880,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>26</v>
@@ -3902,16 +3892,16 @@
         <v>522004</v>
       </c>
       <c r="G31">
-        <v>915</v>
+        <v>902</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>26</v>
@@ -3921,7 +3911,7 @@
         <v>1</v>
       </c>
       <c r="O31">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="3">
@@ -3934,7 +3924,7 @@
         <v>38353</v>
       </c>
       <c r="U31" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V31" s="2"/>
       <c r="W31">
@@ -3947,7 +3937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>23</v>
       </c>
@@ -3955,7 +3945,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>26</v>
@@ -3973,10 +3963,10 @@
         <v>27</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>26</v>
@@ -3986,7 +3976,7 @@
         <v>1</v>
       </c>
       <c r="O32">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="3">
@@ -3999,7 +3989,7 @@
         <v>38353</v>
       </c>
       <c r="U32" s="3">
-        <v>45318.045695577763</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V32" s="2"/>
       <c r="W32">
@@ -4012,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4020,7 +4010,7 @@
         <v>43</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>26</v>
@@ -4038,10 +4028,10 @@
         <v>27</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>26</v>
@@ -4051,7 +4041,7 @@
         <v>1</v>
       </c>
       <c r="O33">
-        <v>25208</v>
+        <v>25186</v>
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="3">
@@ -4064,7 +4054,7 @@
         <v>37987</v>
       </c>
       <c r="U33" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V33" s="2"/>
       <c r="W33">
@@ -4077,7 +4067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>3</v>
       </c>
@@ -4085,7 +4075,7 @@
         <v>44</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>26</v>
@@ -4100,13 +4090,13 @@
         <v>365</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>26</v>
@@ -4129,7 +4119,7 @@
         <v>38718</v>
       </c>
       <c r="U34" s="3">
-        <v>45318.045695566172</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V34" s="2"/>
       <c r="W34">
@@ -4142,7 +4132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2</v>
       </c>
@@ -4150,7 +4140,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>26</v>
@@ -4165,13 +4155,13 @@
         <v>765</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>26</v>
@@ -4194,7 +4184,7 @@
         <v>35065</v>
       </c>
       <c r="U35" s="3">
-        <v>45318.045695566172</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V35" s="2"/>
       <c r="W35">
@@ -4207,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>37</v>
       </c>
@@ -4215,7 +4205,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>26</v>
@@ -4233,10 +4223,10 @@
         <v>27</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>26</v>
@@ -4246,7 +4236,7 @@
         <v>1</v>
       </c>
       <c r="O36">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="3">
@@ -4259,7 +4249,7 @@
         <v>38353</v>
       </c>
       <c r="U36" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512056873</v>
       </c>
       <c r="V36" s="2"/>
       <c r="W36">
@@ -4272,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>38</v>
       </c>
@@ -4280,7 +4270,7 @@
         <v>28</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>26</v>
@@ -4298,10 +4288,10 @@
         <v>27</v>
       </c>
       <c r="I37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>26</v>
@@ -4311,7 +4301,7 @@
         <v>1</v>
       </c>
       <c r="O37">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="3">
@@ -4324,7 +4314,7 @@
         <v>35065</v>
       </c>
       <c r="U37" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512067569</v>
       </c>
       <c r="V37" s="2"/>
       <c r="W37">
@@ -4337,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>41</v>
       </c>
@@ -4345,7 +4335,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>26</v>
@@ -4363,10 +4353,10 @@
         <v>27</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>26</v>
@@ -4376,7 +4366,7 @@
         <v>1</v>
       </c>
       <c r="O38">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="3">
@@ -4389,7 +4379,7 @@
         <v>38718</v>
       </c>
       <c r="U38" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512067569</v>
       </c>
       <c r="V38" s="2"/>
       <c r="W38">
@@ -4402,7 +4392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>39</v>
       </c>
@@ -4410,7 +4400,7 @@
         <v>34</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>26</v>
@@ -4422,16 +4412,16 @@
         <v>395001</v>
       </c>
       <c r="G39">
-        <v>1421</v>
+        <v>1099</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>26</v>
@@ -4441,7 +4431,7 @@
         <v>1</v>
       </c>
       <c r="O39">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q39" s="2"/>
       <c r="R39" s="3">
@@ -4454,7 +4444,7 @@
         <v>38718</v>
       </c>
       <c r="U39" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512067569</v>
       </c>
       <c r="V39" s="2"/>
       <c r="W39">
@@ -4467,7 +4457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>44</v>
       </c>
@@ -4475,7 +4465,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>26</v>
@@ -4493,10 +4483,10 @@
         <v>27</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>26</v>
@@ -4506,7 +4496,7 @@
         <v>1</v>
       </c>
       <c r="O40">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q40" s="2"/>
       <c r="R40" s="3">
@@ -4519,7 +4509,7 @@
         <v>38718</v>
       </c>
       <c r="U40" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512067569</v>
       </c>
       <c r="V40" s="2"/>
       <c r="W40">
@@ -4532,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>42</v>
       </c>
@@ -4540,7 +4530,7 @@
         <v>37</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>26</v>
@@ -4558,10 +4548,10 @@
         <v>27</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>26</v>
@@ -4571,7 +4561,7 @@
         <v>1</v>
       </c>
       <c r="O41">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="3">
@@ -4584,7 +4574,7 @@
         <v>37987</v>
       </c>
       <c r="U41" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512067569</v>
       </c>
       <c r="V41" s="2"/>
       <c r="W41">
@@ -4597,7 +4587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4605,7 +4595,7 @@
         <v>35</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>26</v>
@@ -4623,10 +4613,10 @@
         <v>27</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>26</v>
@@ -4636,7 +4626,7 @@
         <v>1</v>
       </c>
       <c r="O42">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="3">
@@ -4649,7 +4639,7 @@
         <v>38718</v>
       </c>
       <c r="U42" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512067569</v>
       </c>
       <c r="V42" s="2"/>
       <c r="W42">
@@ -4662,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>4</v>
       </c>
@@ -4670,7 +4660,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>26</v>
@@ -4685,13 +4675,13 @@
         <v>562</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>26</v>
@@ -4714,7 +4704,7 @@
         <v>38353</v>
       </c>
       <c r="U43" s="3">
-        <v>45318.045695566172</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V43" s="2"/>
       <c r="W43">
@@ -4727,7 +4717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>5</v>
       </c>
@@ -4735,7 +4725,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>26</v>
@@ -4750,13 +4740,13 @@
         <v>779</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>26</v>
@@ -4779,7 +4769,7 @@
         <v>38353</v>
       </c>
       <c r="U44" s="3">
-        <v>45318.045695566172</v>
+        <v>45459.706512044337</v>
       </c>
       <c r="V44" s="2"/>
       <c r="W44">
@@ -4792,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>45</v>
       </c>
@@ -4800,7 +4790,7 @@
         <v>41</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>26</v>
@@ -4812,16 +4802,16 @@
         <v>255980</v>
       </c>
       <c r="G45">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>26</v>
@@ -4831,7 +4821,7 @@
         <v>1</v>
       </c>
       <c r="O45">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="3">
@@ -4844,7 +4834,7 @@
         <v>38718</v>
       </c>
       <c r="U45" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512067569</v>
       </c>
       <c r="V45" s="2"/>
       <c r="W45">
@@ -4857,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>46</v>
       </c>
@@ -4865,7 +4855,7 @@
         <v>42</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>26</v>
@@ -4883,10 +4873,10 @@
         <v>27</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>26</v>
@@ -4896,7 +4886,7 @@
         <v>1</v>
       </c>
       <c r="O46">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q46" s="2"/>
       <c r="R46" s="3">
@@ -4909,7 +4899,7 @@
         <v>38353</v>
       </c>
       <c r="U46" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512067569</v>
       </c>
       <c r="V46" s="2"/>
       <c r="W46">
@@ -4922,7 +4912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>43</v>
       </c>
@@ -4930,7 +4920,7 @@
         <v>38</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>26</v>
@@ -4948,10 +4938,10 @@
         <v>27</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>26</v>
@@ -4961,7 +4951,7 @@
         <v>1</v>
       </c>
       <c r="O47">
-        <v>9589</v>
+        <v>9265</v>
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="3">
@@ -4974,7 +4964,7 @@
         <v>37987</v>
       </c>
       <c r="U47" s="3">
-        <v>45318.045695589317</v>
+        <v>45459.706512067569</v>
       </c>
       <c r="V47" s="2"/>
       <c r="W47">

</xml_diff>